<commit_message>
LatestChanged and resolved issues
</commit_message>
<xml_diff>
--- a/DemoProject/src/test/java/com/demo/testdata/web/testdata.xlsx
+++ b/DemoProject/src/test/java/com/demo/testdata/web/testdata.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="2"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="Login" sheetId="1" state="visible" r:id="rId2"/>
@@ -174,13 +174,13 @@
     <t xml:space="preserve">ARTHROSCOPIC STABILISATION PROCEDURE</t>
   </si>
   <si>
-    <t xml:space="preserve">Test1001</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Eat more fiber</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Procedure1001</t>
+    <t xml:space="preserve">Created test</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Created instructions</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Procedure created</t>
   </si>
   <si>
     <t xml:space="preserve">Records Date</t>
@@ -189,7 +189,7 @@
     <t xml:space="preserve">Todays Date</t>
   </si>
   <si>
-    <t xml:space="preserve">Jul 7, 2023</t>
+    <t xml:space="preserve">Aug 10, 2023</t>
   </si>
   <si>
     <t xml:space="preserve">Mobile No</t>
@@ -380,13 +380,13 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:B21"/>
+  <dimension ref="A1:B1000"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="1" sqref="B2 A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.4375" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="14.453125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="14.29"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="17.29"/>
@@ -1409,13 +1409,13 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:D3"/>
+  <dimension ref="A1:D1000"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="1" sqref="B2 A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.4375" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="14.453125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="14.14"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="17.43"/>
@@ -2466,13 +2466,13 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:N3"/>
+  <dimension ref="A1:N1000"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C2" activeCellId="0" sqref="C2"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C2" activeCellId="1" sqref="B2 C2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.4375" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="14.453125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="23"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="18.29"/>
@@ -3592,19 +3592,19 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:F3"/>
+  <dimension ref="A1:F1000"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="D1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F2" activeCellId="0" sqref="F2"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="E2" activeCellId="1" sqref="B2 E2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.4375" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="14.453125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="12"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="18.43"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="37"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="18.74"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="5" style="0" width="21.05"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="5" style="0" width="21.04"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="26" min="7" style="0" width="9.14"/>
   </cols>
   <sheetData>
@@ -4664,11 +4664,11 @@
   </sheetPr>
   <dimension ref="A1:B2"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B12" activeCellId="0" sqref="B12"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B2" activeCellId="0" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.14453125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="9.16015625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="12.01"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="13.34"/>
@@ -4709,12 +4709,12 @@
   <dimension ref="A1:B2"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B12" activeCellId="0" sqref="B12"/>
+      <selection pane="topLeft" activeCell="B12" activeCellId="1" sqref="B2 B12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.14453125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="9.16015625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="17.97"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="17.98"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="21.28"/>
   </cols>
   <sheetData>

</xml_diff>